<commit_message>
Amy cleaning up and expanding code for wilcox signed rank tests of slopes
</commit_message>
<xml_diff>
--- a/Genomics_scripts/Data/wilcox_slope_p-values.xlsx
+++ b/Genomics_scripts/Data/wilcox_slope_p-values.xlsx
@@ -1,26 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/AM_Workshop/AM_Workshop/Genomics_scripts/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amyangert/Documents/Git clones/AM_Workshop/Genomics_scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9F559405-3879-7047-A526-B4C69D089522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6355C70-758C-2046-8778-F8EA03A34DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="18680" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="wilcox_slope_p-values" sheetId="1" r:id="rId1"/>
+    <sheet name="full vectors" sheetId="1" r:id="rId1"/>
+    <sheet name="trimmed to -2,2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Amy Angert</author>
+  </authors>
+  <commentList>
+    <comment ref="AC13" authorId="0" shapeId="0" xr:uid="{304DBC11-677B-1F4D-BE3F-0398F240A14F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amy Angert:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>this one doesn't make sense</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
   <si>
     <t>MAT</t>
   </si>
@@ -111,15 +155,37 @@
   <si>
     <t>S15</t>
   </si>
+  <si>
+    <t>one-tailed (&gt;0)</t>
+  </si>
+  <si>
+    <t>two-tailed (=/= 0)</t>
+  </si>
+  <si>
+    <t>one-tailed (&lt;0)</t>
+  </si>
+  <si>
+    <t>CLIMATE-ASSOCIATED LOCI</t>
+  </si>
+  <si>
+    <t>RANDOM LOCI</t>
+  </si>
+  <si>
+    <t>TWO-SAMPLE CLIM vs RAND</t>
+  </si>
+  <si>
+    <t>one-tailed (clim&gt;rand)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -254,8 +320,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +540,24 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -596,7 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,12 +727,57 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -657,6 +825,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8C7C8F"/>
+      <color rgb="FF8C5F91"/>
+      <color rgb="FFE8D952"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -964,276 +1139,2520 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5.5" customWidth="1"/>
+    <col min="13" max="14" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" customWidth="1"/>
+    <col min="17" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.33203125" customWidth="1"/>
+    <col min="20" max="20" width="5.33203125" customWidth="1"/>
+    <col min="21" max="22" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3" customWidth="1"/>
+    <col min="24" max="24" width="5.33203125" customWidth="1"/>
+    <col min="25" max="26" width="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5" customWidth="1"/>
+    <col min="28" max="28" width="8.5" customWidth="1"/>
+    <col min="29" max="30" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
         <v>7.56714E-2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E4" s="2">
         <v>0.40098361999999999</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F4" s="2">
         <v>0.73453186000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="H4" s="13">
+        <v>0.1513428</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0.80196719999999999</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0.53137509999999999</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.92443960000000003</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.5991166</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.26568750000000002</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="12">
+        <v>7.4899504748317296E-12</v>
+      </c>
+      <c r="U4" s="12">
+        <v>1.6890649196538399E-12</v>
+      </c>
+      <c r="V4" s="12">
+        <v>2.8519785811025799E-30</v>
+      </c>
+      <c r="X4" s="9">
+        <v>3.744975E-12</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>8.4453249999999997E-13</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>1.425989E-30</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB4" s="31">
+        <v>1.527906E-12</v>
+      </c>
+      <c r="AC4" s="32">
+        <v>1.527906E-12</v>
+      </c>
+      <c r="AD4" s="32">
+        <v>1.272922E-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C5" s="1">
         <v>12</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D5" s="8">
         <v>5.3210499999999999E-3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E5" s="8">
         <v>1.3500000000000001E-17</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F5" s="2">
         <v>0.92902470000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="H5" s="13">
+        <v>1.06421E-2</v>
+      </c>
+      <c r="I5" s="13">
+        <v>2.7034760000000001E-17</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0.14214399999999999</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.99469149999999995</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="9">
+        <v>7.107202E-2</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.77504119999999999</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0.5683262</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0.86164850000000004</v>
+      </c>
+      <c r="T5" s="11">
+        <v>0.45148982778904201</v>
+      </c>
+      <c r="U5" s="11">
+        <v>0.864087066707806</v>
+      </c>
+      <c r="V5" s="11">
+        <v>0.27771876549227498</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0.2257449</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>0.43204350000000002</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>0.13885939999999999</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="31">
+        <v>9.8795700000000007E-3</v>
+      </c>
+      <c r="AC5" s="31">
+        <v>9.8795700000000007E-3</v>
+      </c>
+      <c r="AD5" s="33">
+        <v>0.99590259999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D6" s="2">
         <v>0.99997462999999998</v>
       </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
         <v>6.9400000000000006E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="H6" s="16">
+        <v>5.0918860000000002E-5</v>
+      </c>
+      <c r="I6" s="16">
+        <v>4.036536E-16</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1.3881019999999999E-4</v>
+      </c>
+      <c r="L6" s="9">
+        <v>2.5459430000000001E-5</v>
+      </c>
+      <c r="M6" s="9">
+        <v>2.018268E-16</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.99993080000000001</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0.98197699999999999</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0.80344300000000002</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1</v>
+      </c>
+      <c r="T6" s="12">
+        <v>3.6179425969931803E-2</v>
+      </c>
+      <c r="U6" s="11">
+        <v>0.39338982697055003</v>
+      </c>
+      <c r="V6" s="12">
+        <v>1.65292545193084E-12</v>
+      </c>
+      <c r="X6" s="9">
+        <v>1.8089709999999998E-2</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>0.19669490000000001</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>8.2646270000000004E-13</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="33">
+        <v>0.86747209999999997</v>
+      </c>
+      <c r="AC6" s="33">
+        <v>0.86747209999999997</v>
+      </c>
+      <c r="AD6" s="31">
+        <v>4.0356290000000001E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D7" s="8">
         <v>2.5900000000000001E-4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E7" s="8">
         <v>9.1199999999999999E-9</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F7" s="2">
         <v>0.99992453000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="H7" s="17">
+        <v>5.1740309999999997E-4</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1.8249669999999999E-8</v>
+      </c>
+      <c r="J7" s="16">
+        <v>1.5134879999999999E-4</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.99974200000000002</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="9">
+        <v>7.5674399999999995E-5</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="12">
+        <v>1.5565964547345801E-14</v>
+      </c>
+      <c r="U7" s="12">
+        <v>6.8792578174337799E-14</v>
+      </c>
+      <c r="V7" s="12">
+        <v>8.0748943662228804E-14</v>
+      </c>
+      <c r="X7" s="9">
+        <v>7.7829820000000005E-15</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>3.4396290000000003E-14</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>4.0374469999999999E-14</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB7" s="31">
+        <v>1.528184E-16</v>
+      </c>
+      <c r="AC7" s="31">
+        <v>1.528184E-16</v>
+      </c>
+      <c r="AD7" s="32">
+        <v>1.5279459999999999E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D8" s="8">
         <v>2.7442600000000001E-3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E8" s="7">
         <v>4.9985399999999999E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F8" s="2">
         <v>0.97925711000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="H8" s="17">
+        <v>5.488527E-3</v>
+      </c>
+      <c r="I8" s="13">
+        <v>9.9970799999999999E-2</v>
+      </c>
+      <c r="J8" s="16">
+        <v>4.1552939999999997E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.99726219999999999</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.95004089999999997</v>
+      </c>
+      <c r="N8" s="9">
+        <v>2.0776469999999998E-2</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="T8" s="12">
+        <v>3.1634248983708802E-17</v>
+      </c>
+      <c r="U8" s="12">
+        <v>9.8307917987510599E-23</v>
+      </c>
+      <c r="V8" s="12">
+        <v>3.3815654428916699E-23</v>
+      </c>
+      <c r="X8" s="9">
+        <v>1.5817120000000001E-17</v>
+      </c>
+      <c r="Y8" s="9">
+        <v>4.9153959999999999E-23</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>1.690783E-23</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB8" s="31">
+        <v>1.352811E-19</v>
+      </c>
+      <c r="AC8" s="31">
+        <v>1.352811E-19</v>
+      </c>
+      <c r="AD8" s="32">
+        <v>3.8408360000000002E-14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C9" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D9" s="2">
         <v>0.79501664000000005</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E9" s="2">
         <v>0.99998370000000003</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F9" s="7">
         <v>2.1066430000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="H9" s="14">
+        <v>0.4104024</v>
+      </c>
+      <c r="I9" s="16">
+        <v>3.2637859999999999E-5</v>
+      </c>
+      <c r="J9" s="17">
+        <v>4.2132860000000001E-2</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.2052012</v>
+      </c>
+      <c r="M9" s="9">
+        <v>1.6318929999999999E-5</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.97896689999999997</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.99999939999999998</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.99992239999999999</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.99999680000000002</v>
+      </c>
+      <c r="T9" s="12">
+        <v>1.2584857167320101E-6</v>
+      </c>
+      <c r="U9" s="12">
+        <v>1.5543507143204601E-4</v>
+      </c>
+      <c r="V9" s="12">
+        <v>6.4558238614694698E-6</v>
+      </c>
+      <c r="X9" s="9">
+        <v>6.2924290000000003E-7</v>
+      </c>
+      <c r="Y9" s="9">
+        <v>7.7717539999999999E-5</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>3.227912E-6</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB9" s="32">
+        <v>2.9169540000000002E-6</v>
+      </c>
+      <c r="AC9" s="32">
+        <v>2.9169540000000002E-6</v>
+      </c>
+      <c r="AD9" s="31">
+        <v>5.568925E-10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C10" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D10" s="2">
         <v>0.13288261000000001</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E10" s="2">
         <v>0.99988953000000003</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F10" s="8">
         <v>3.5399999999999999E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="H10" s="14">
+        <v>0.26576519999999998</v>
+      </c>
+      <c r="I10" s="16">
+        <v>2.211584E-4</v>
+      </c>
+      <c r="J10" s="17">
+        <v>7.0759209999999998E-4</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.8672858</v>
+      </c>
+      <c r="M10" s="9">
+        <v>1.105792E-4</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.99964710000000001</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1</v>
+      </c>
+      <c r="R10" s="4">
+        <v>1</v>
+      </c>
+      <c r="T10" s="12">
+        <v>2.1041564780395E-11</v>
+      </c>
+      <c r="U10" s="12">
+        <v>2.50150066470522E-22</v>
+      </c>
+      <c r="V10" s="12">
+        <v>5.2136910806337104E-9</v>
+      </c>
+      <c r="X10" s="9">
+        <v>1.0520780000000001E-11</v>
+      </c>
+      <c r="Y10" s="9">
+        <v>1.2507499999999999E-22</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>2.6068459999999999E-9</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB10" s="32">
+        <v>8.0847210000000003E-8</v>
+      </c>
+      <c r="AC10" s="32">
+        <v>8.0847210000000003E-8</v>
+      </c>
+      <c r="AD10" s="31">
+        <v>9.9508879999999997E-14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D11" s="2">
         <v>0.99999996000000002</v>
       </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
         <v>1.3719100000000001E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="H11" s="16">
+        <v>7.091198E-8</v>
+      </c>
+      <c r="I11" s="16">
+        <v>3.3434699999999999E-15</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2.7438240000000002E-3</v>
+      </c>
+      <c r="L11" s="9">
+        <v>3.545599E-8</v>
+      </c>
+      <c r="M11" s="9">
+        <v>1.6717349999999999E-15</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0.99863109999999999</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0.99999910000000003</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0.99998960000000003</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0.74992219999999998</v>
+      </c>
+      <c r="T11" s="12">
+        <v>1.85282705748061E-6</v>
+      </c>
+      <c r="U11" s="12">
+        <v>2.0845005502281202E-5</v>
+      </c>
+      <c r="V11" s="11">
+        <v>0.50084717953846003</v>
+      </c>
+      <c r="X11" s="9">
+        <v>9.2641349999999999E-7</v>
+      </c>
+      <c r="Y11" s="9">
+        <v>1.0422500000000001E-5</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>0.25042360000000002</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB11" s="32">
+        <v>1.4850729999999999E-2</v>
+      </c>
+      <c r="AC11" s="32">
+        <v>1.4850729999999999E-2</v>
+      </c>
+      <c r="AD11" s="31">
+        <v>1.5976160000000002E-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D12" s="2">
         <v>3.0502609999999999E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E12" s="2">
         <v>0.98612668999999997</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F12" s="8">
         <v>1.5799999999999999E-9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="H12" s="16">
+        <v>6.1005230000000001E-2</v>
+      </c>
+      <c r="I12" s="16">
+        <v>2.7765430000000001E-2</v>
+      </c>
+      <c r="J12" s="17">
+        <v>3.1545389999999998E-9</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.96955429999999998</v>
+      </c>
+      <c r="M12" s="9">
+        <v>1.3882709999999999E-2</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="P12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>1</v>
+      </c>
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="T12" s="12">
+        <v>1.23768073321268E-11</v>
+      </c>
+      <c r="U12" s="12">
+        <v>1.1190865216411501E-16</v>
+      </c>
+      <c r="V12" s="12">
+        <v>1.3112029340802899E-12</v>
+      </c>
+      <c r="X12" s="9">
+        <v>6.1884039999999996E-12</v>
+      </c>
+      <c r="Y12" s="9">
+        <v>5.5954329999999999E-17</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>6.5560150000000001E-13</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB12" s="32">
+        <v>3.3958140000000002E-18</v>
+      </c>
+      <c r="AC12" s="32">
+        <v>3.3958140000000002E-18</v>
+      </c>
+      <c r="AD12" s="31">
+        <v>1.1278330000000001E-28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>9</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D13" s="2">
         <v>0.99787373999999995</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E13" s="8">
         <v>1.17E-4</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F13" s="2">
         <v>0.99942076999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="H13" s="16">
+        <v>4.2628049999999997E-3</v>
+      </c>
+      <c r="I13" s="17">
+        <v>2.3488679999999999E-4</v>
+      </c>
+      <c r="J13" s="16">
+        <v>1.1611390000000001E-3</v>
+      </c>
+      <c r="L13" s="9">
+        <v>2.1314020000000001E-3</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0.99988270000000001</v>
+      </c>
+      <c r="N13" s="9">
+        <v>5.8056950000000003E-4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>1</v>
+      </c>
+      <c r="R13" s="4">
+        <v>0.99877300000000002</v>
+      </c>
+      <c r="T13" s="12">
+        <v>1.4016740563331401E-9</v>
+      </c>
+      <c r="U13" s="12">
+        <v>1.2968464366252601E-14</v>
+      </c>
+      <c r="V13" s="12">
+        <v>2.4637652117114098E-3</v>
+      </c>
+      <c r="X13" s="9">
+        <v>7.0083700000000001E-10</v>
+      </c>
+      <c r="Y13" s="9">
+        <v>6.4842319999999997E-15</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>1.231883E-3</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB13" s="32">
+        <v>2.1959860000000001E-2</v>
+      </c>
+      <c r="AC13" s="31">
+        <v>2.1959860000000001E-2</v>
+      </c>
+      <c r="AD13" s="32">
+        <v>1.0567170000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C14" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D14" s="2">
         <v>0.86548369000000003</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E14" s="2">
         <v>0.273364</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F14" s="2">
         <v>0.53102532999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="H14" s="14">
+        <v>0.26948220000000001</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0.54672799999999999</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.93851490000000004</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.1347411</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.72673359999999998</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.46925739999999999</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0.85833119999999996</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0.75927739999999999</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0.81326960000000004</v>
+      </c>
+      <c r="T14" s="11">
+        <v>0.28393861091476302</v>
+      </c>
+      <c r="U14" s="11">
+        <v>0.481654001891415</v>
+      </c>
+      <c r="V14" s="11">
+        <v>0.37407896586281097</v>
+      </c>
+      <c r="X14" s="4">
+        <v>0.14196929999999999</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>0.24082700000000001</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>0.1870395</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB14" s="33">
+        <v>0.1244165</v>
+      </c>
+      <c r="AC14" s="33">
+        <v>0.1244165</v>
+      </c>
+      <c r="AD14" s="32">
+        <v>9.1842520000000004E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="1">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D15" s="8">
         <v>2.2158600000000001E-3</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E15" s="8">
         <v>2.85E-10</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F15" s="2">
         <v>0.99997798000000004</v>
       </c>
+      <c r="H15" s="17">
+        <v>4.431712E-3</v>
+      </c>
+      <c r="I15" s="17">
+        <v>5.6920540000000002E-10</v>
+      </c>
+      <c r="J15" s="16">
+        <v>4.416168E-5</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.9977895</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="9">
+        <v>2.208084E-5</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0.99785710000000005</v>
+      </c>
+      <c r="T15" s="12">
+        <v>1.2059261699013701E-15</v>
+      </c>
+      <c r="U15" s="12">
+        <v>1.2175976837690399E-41</v>
+      </c>
+      <c r="V15" s="12">
+        <v>4.2978269169047303E-3</v>
+      </c>
+      <c r="X15" s="9">
+        <v>6.0296309999999997E-16</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>6.087988E-42</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>2.1489130000000001E-3</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB15" s="31">
+        <v>9.1060589999999996E-18</v>
+      </c>
+      <c r="AC15" s="31">
+        <v>9.1060589999999996E-18</v>
+      </c>
+      <c r="AD15" s="32">
+        <v>4.2735489999999999E-13</v>
+      </c>
+    </row>
+    <row r="17" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="O18" s="3"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+    </row>
+    <row r="19" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="O19" s="3"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="4"/>
+      <c r="AD19" s="4"/>
+    </row>
+    <row r="20" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+    </row>
+    <row r="21" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+    </row>
+    <row r="22" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+    </row>
+    <row r="23" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+    </row>
+    <row r="24" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+    </row>
+    <row r="25" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+    </row>
+    <row r="26" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+    </row>
+    <row r="27" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+    </row>
+    <row r="28" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+    </row>
+    <row r="29" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+    </row>
+    <row r="30" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+    </row>
+    <row r="31" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA30B2AA-942D-F445-BACB-965CCA47F8FD}">
+  <dimension ref="A1:AD17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.6640625" customWidth="1"/>
+    <col min="12" max="12" width="5.5" customWidth="1"/>
+    <col min="13" max="14" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" customWidth="1"/>
+    <col min="17" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.33203125" customWidth="1"/>
+    <col min="20" max="20" width="5.33203125" customWidth="1"/>
+    <col min="21" max="22" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3" customWidth="1"/>
+    <col min="24" max="24" width="5.33203125" customWidth="1"/>
+    <col min="25" max="26" width="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.5" customWidth="1"/>
+    <col min="28" max="30" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.30905991350000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.86386189999999996</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.77137820000000001</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.6181198</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.27241789999999999</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.45774039999999999</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21">
+        <v>0.69125970000000003</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.136209</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0.22887019820000001</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0.99999894</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0.99998730000000002</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="12">
+        <v>2.1512159999999999E-6</v>
+      </c>
+      <c r="U4" s="12">
+        <v>2.542057E-5</v>
+      </c>
+      <c r="V4" s="12">
+        <v>9.924568E-12</v>
+      </c>
+      <c r="W4" s="20"/>
+      <c r="X4" s="12">
+        <v>1.0756079999999999E-6</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>1.271028E-5</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>4.962284E-12</v>
+      </c>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="26">
+        <v>5.6412759999999999E-6</v>
+      </c>
+      <c r="AC4" s="26">
+        <v>5.6412759999999999E-6</v>
+      </c>
+      <c r="AD4" s="26">
+        <v>1.1195240000000001E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>12</v>
+      </c>
+      <c r="D5" s="23">
+        <v>3.5178520200000001E-2</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1.8955110000000001E-15</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.76355989999999996</v>
+      </c>
+      <c r="H5" s="30">
+        <v>7.0357039999999996E-2</v>
+      </c>
+      <c r="I5" s="30">
+        <v>3.7910209999999996E-15</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.4733542</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21">
+        <v>0.9648892</v>
+      </c>
+      <c r="M5" s="21">
+        <v>1</v>
+      </c>
+      <c r="N5" s="21">
+        <v>0.23667712420000001</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.98752251000000002</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0.73930640000000003</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0.91971053000000003</v>
+      </c>
+      <c r="T5" s="12">
+        <v>2.5220570000000001E-2</v>
+      </c>
+      <c r="U5" s="11">
+        <v>0.52237239999999996</v>
+      </c>
+      <c r="V5" s="11">
+        <v>0.1617623</v>
+      </c>
+      <c r="W5" s="20"/>
+      <c r="X5" s="12">
+        <v>1.261028E-2</v>
+      </c>
+      <c r="Y5" s="11">
+        <v>0.26118619999999998</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>8.0881149999999999E-2</v>
+      </c>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="23">
+        <v>7.366666E-3</v>
+      </c>
+      <c r="AC5" s="23">
+        <v>7.366666E-3</v>
+      </c>
+      <c r="AD5" s="22">
+        <v>0.97712410000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.99997474659999996</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.99999629999999995</v>
+      </c>
+      <c r="F6" s="23">
+        <v>1.4371519999999999E-3</v>
+      </c>
+      <c r="H6" s="12">
+        <v>5.0717460000000001E-5</v>
+      </c>
+      <c r="I6" s="12">
+        <v>7.4474930000000003E-6</v>
+      </c>
+      <c r="J6" s="30">
+        <v>2.8743050000000002E-3</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="16">
+        <v>2.535873E-5</v>
+      </c>
+      <c r="M6" s="16">
+        <v>3.723746E-6</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0.99856707840000003</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0.74568396999999997</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0.86546749999999995</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0.99996671000000004</v>
+      </c>
+      <c r="T6" s="11">
+        <v>0.51077530000000004</v>
+      </c>
+      <c r="U6" s="11">
+        <v>0.26948040000000001</v>
+      </c>
+      <c r="V6" s="12">
+        <v>6.7254649999999995E-5</v>
+      </c>
+      <c r="W6" s="20"/>
+      <c r="X6" s="19">
+        <v>0.25538759999999999</v>
+      </c>
+      <c r="Y6" s="19">
+        <v>0.1347402</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>3.3627329999999998E-5</v>
+      </c>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="22">
+        <v>0.99723729999999999</v>
+      </c>
+      <c r="AC6" s="22">
+        <v>0.99723729999999999</v>
+      </c>
+      <c r="AD6" s="23">
+        <v>6.8313650000000005E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="23">
+        <v>8.7377449999999997E-4</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1.188477E-4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.99447660000000004</v>
+      </c>
+      <c r="H7" s="30">
+        <v>1.7475489999999999E-3</v>
+      </c>
+      <c r="I7" s="30">
+        <v>2.3769549999999999E-4</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1.107173E-2</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21">
+        <v>0.99912880000000004</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.99988129999999997</v>
+      </c>
+      <c r="N7" s="16">
+        <v>5.5358626999999997E-3</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0.98668365999999996</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0.99999979999999999</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0.99988334000000001</v>
+      </c>
+      <c r="T7" s="12">
+        <v>2.7003139999999998E-2</v>
+      </c>
+      <c r="U7" s="12">
+        <v>3.112174E-7</v>
+      </c>
+      <c r="V7" s="12">
+        <v>2.3758279999999999E-4</v>
+      </c>
+      <c r="W7" s="20"/>
+      <c r="X7" s="12">
+        <v>1.3501569999999999E-2</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>1.556087E-7</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>1.187914E-4</v>
+      </c>
+      <c r="AA7" s="24"/>
+      <c r="AB7" s="23">
+        <v>2.7143780000000003E-4</v>
+      </c>
+      <c r="AC7" s="23">
+        <v>2.7143780000000003E-4</v>
+      </c>
+      <c r="AD7" s="22">
+        <v>0.49477710000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="23">
+        <v>4.5009650499999998E-2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.25831569999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.95767290000000005</v>
+      </c>
+      <c r="H8" s="30">
+        <v>9.0019299999999997E-2</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.51663130000000002</v>
+      </c>
+      <c r="J8" s="12">
+        <v>8.4789619999999996E-2</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21">
+        <v>0.95506979999999997</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.74177570000000004</v>
+      </c>
+      <c r="N8" s="16">
+        <v>4.2394807600000001E-2</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.91488053000000003</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0.99978</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.99999203999999997</v>
+      </c>
+      <c r="T8" s="19">
+        <v>0.17219380000000001</v>
+      </c>
+      <c r="U8" s="12">
+        <v>4.4177220000000001E-4</v>
+      </c>
+      <c r="V8" s="12">
+        <v>1.618003E-5</v>
+      </c>
+      <c r="W8" s="20"/>
+      <c r="X8" s="12">
+        <v>8.6096909999999999E-2</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>2.2088610000000001E-4</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>8.0900170000000003E-6</v>
+      </c>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="23">
+        <v>1.1817609999999999E-2</v>
+      </c>
+      <c r="AC8" s="26">
+        <v>1.1817609999999999E-2</v>
+      </c>
+      <c r="AD8" s="22">
+        <v>0.338642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.42529618940000002</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.99987230000000005</v>
+      </c>
+      <c r="F9" s="23">
+        <v>8.0736920000000004E-2</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.85059240000000003</v>
+      </c>
+      <c r="I9" s="12">
+        <v>2.5574499999999998E-4</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.1614738</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21">
+        <v>0.57505280000000003</v>
+      </c>
+      <c r="M9" s="16">
+        <v>1.2787249999999999E-4</v>
+      </c>
+      <c r="N9" s="21">
+        <v>0.91937230619999999</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.99992130000000001</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.83728360000000002</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.99922049000000002</v>
+      </c>
+      <c r="T9" s="12">
+        <v>1.593245E-4</v>
+      </c>
+      <c r="U9" s="19">
+        <v>0.3259264</v>
+      </c>
+      <c r="V9" s="12">
+        <v>1.57346E-3</v>
+      </c>
+      <c r="W9" s="20"/>
+      <c r="X9" s="12">
+        <v>7.966223E-5</v>
+      </c>
+      <c r="Y9" s="19">
+        <v>0.1629632</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>7.8672989999999999E-4</v>
+      </c>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="26">
+        <v>2.85961E-4</v>
+      </c>
+      <c r="AC9" s="26">
+        <v>2.85961E-4</v>
+      </c>
+      <c r="AD9" s="23">
+        <v>1.274853E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.15459698999999999</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.99995230000000002</v>
+      </c>
+      <c r="F10" s="23">
+        <v>8.2099210000000002E-5</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.30919400000000002</v>
+      </c>
+      <c r="I10" s="12">
+        <v>9.5571419999999999E-5</v>
+      </c>
+      <c r="J10" s="30">
+        <v>1.641984E-4</v>
+      </c>
+      <c r="K10" s="20"/>
+      <c r="L10" s="21">
+        <v>0.84560990000000003</v>
+      </c>
+      <c r="M10" s="16">
+        <v>4.778571E-5</v>
+      </c>
+      <c r="N10" s="21">
+        <v>0.99991814059999995</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0.97835528999999999</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.98320107999999995</v>
+      </c>
+      <c r="T10" s="12">
+        <v>4.3817849999999998E-2</v>
+      </c>
+      <c r="U10" s="12">
+        <v>1.4909409999999999E-9</v>
+      </c>
+      <c r="V10" s="12">
+        <v>3.3899329999999998E-2</v>
+      </c>
+      <c r="W10" s="20"/>
+      <c r="X10" s="12">
+        <v>2.1908919999999998E-2</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>7.454706E-10</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>1.6949659999999998E-2</v>
+      </c>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="26">
+        <v>9.2153520000000003E-2</v>
+      </c>
+      <c r="AC10" s="26">
+        <v>9.2153520000000003E-2</v>
+      </c>
+      <c r="AD10" s="23">
+        <v>9.1538530000000003E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.99989012749999995</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.6501709</v>
+      </c>
+      <c r="H11" s="12">
+        <v>2.2064750000000001E-4</v>
+      </c>
+      <c r="I11" s="12">
+        <v>1.5554229999999999E-9</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.70027340000000005</v>
+      </c>
+      <c r="K11" s="20"/>
+      <c r="L11" s="16">
+        <v>1.103237E-4</v>
+      </c>
+      <c r="M11" s="16">
+        <v>7.7771170000000002E-10</v>
+      </c>
+      <c r="N11" s="21">
+        <v>0.35013671439999999</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0.97684104000000005</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0.99098339999999996</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0.27658253999999999</v>
+      </c>
+      <c r="T11" s="12">
+        <v>4.6827010000000002E-2</v>
+      </c>
+      <c r="U11" s="12">
+        <v>1.8076120000000001E-2</v>
+      </c>
+      <c r="V11" s="11">
+        <v>0.55316509999999997</v>
+      </c>
+      <c r="W11" s="20"/>
+      <c r="X11" s="12">
+        <v>2.34135E-2</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>9.0380619999999995E-3</v>
+      </c>
+      <c r="Z11" s="19">
+        <v>0.72437530000000006</v>
+      </c>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="22">
+        <v>0.22034280000000001</v>
+      </c>
+      <c r="AC11" s="22">
+        <v>0.22034280000000001</v>
+      </c>
+      <c r="AD11" s="22">
+        <v>0.17414450000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8</v>
+      </c>
+      <c r="D12" s="23">
+        <v>7.0128919999999997E-4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.87719780000000003</v>
+      </c>
+      <c r="F12" s="23">
+        <v>1.165084E-5</v>
+      </c>
+      <c r="H12" s="30">
+        <v>1.402578E-3</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.2457461</v>
+      </c>
+      <c r="J12" s="30">
+        <v>2.330169E-5</v>
+      </c>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21">
+        <v>0.99930129999999995</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0.1228731</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0.99998839669999995</v>
+      </c>
+      <c r="P12" s="23">
+        <v>6.3068029999999997E-2</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>6.5509219999999996E-6</v>
+      </c>
+      <c r="R12" s="23">
+        <v>3.0698179999999999E-2</v>
+      </c>
+      <c r="T12" s="19">
+        <v>0.1261361</v>
+      </c>
+      <c r="U12" s="30">
+        <v>1.310184E-5</v>
+      </c>
+      <c r="V12" s="30">
+        <v>6.1396369999999999E-2</v>
+      </c>
+      <c r="W12" s="20"/>
+      <c r="X12" s="19">
+        <v>0.93823239999999997</v>
+      </c>
+      <c r="Y12" s="19">
+        <v>0.99999360000000004</v>
+      </c>
+      <c r="Z12" s="19">
+        <v>0.97025740000000005</v>
+      </c>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="23">
+        <v>1.136757E-8</v>
+      </c>
+      <c r="AC12" s="26">
+        <v>1.136757E-8</v>
+      </c>
+      <c r="AD12" s="23">
+        <v>1.6093669999999999E-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.99997131350000001</v>
+      </c>
+      <c r="E13" s="23">
+        <v>7.8605819999999997E-6</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.9993339</v>
+      </c>
+      <c r="H13" s="12">
+        <v>5.7572109999999998E-5</v>
+      </c>
+      <c r="I13" s="30">
+        <v>1.5721159999999998E-5</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1.3354300000000001E-3</v>
+      </c>
+      <c r="K13" s="20"/>
+      <c r="L13" s="16">
+        <v>2.8786059999999999E-5</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.99999210000000005</v>
+      </c>
+      <c r="N13" s="16">
+        <v>6.6771479999999997E-4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0.99005489999999996</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>0.99990259999999997</v>
+      </c>
+      <c r="R13" s="4">
+        <v>0.95669601000000004</v>
+      </c>
+      <c r="T13" s="12">
+        <v>2.0013800000000002E-2</v>
+      </c>
+      <c r="U13" s="12">
+        <v>1.9521149999999999E-4</v>
+      </c>
+      <c r="V13" s="12">
+        <v>8.702153E-2</v>
+      </c>
+      <c r="W13" s="20"/>
+      <c r="X13" s="12">
+        <v>1.0006900000000001E-2</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>9.7605749999999996E-5</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>4.3510769999999997E-2</v>
+      </c>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="22">
+        <v>0.98949220000000004</v>
+      </c>
+      <c r="AC13" s="25">
+        <v>0.98949220000000004</v>
+      </c>
+      <c r="AD13" s="22">
+        <v>0.89259759999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.98602515690000003</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.56182509999999997</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.10534880000000001</v>
+      </c>
+      <c r="H14" s="12">
+        <v>2.8035529999999999E-2</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.87658939999999996</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.21069769999999999</v>
+      </c>
+      <c r="K14" s="20"/>
+      <c r="L14" s="16">
+        <v>1.4017770000000001E-2</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0.43829469999999998</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0.89480050249999998</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0.82893094</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0.98336990000000002</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0.98883151000000002</v>
+      </c>
+      <c r="T14" s="11">
+        <v>0.34325539999999999</v>
+      </c>
+      <c r="U14" s="12">
+        <v>3.3299240000000001E-2</v>
+      </c>
+      <c r="V14" s="12">
+        <v>2.2439069999999998E-2</v>
+      </c>
+      <c r="W14" s="20"/>
+      <c r="X14" s="19">
+        <v>0.17162769999999999</v>
+      </c>
+      <c r="Y14" s="12">
+        <v>1.664962E-2</v>
+      </c>
+      <c r="Z14" s="12">
+        <v>1.121953E-2</v>
+      </c>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="22">
+        <v>0.2654358</v>
+      </c>
+      <c r="AC14" s="22">
+        <v>0.2654358</v>
+      </c>
+      <c r="AD14" s="26">
+        <v>1.83833E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4">
+        <v>9.51366721E-2</v>
+      </c>
+      <c r="E15" s="23">
+        <v>8.7113670000000006E-9</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.99987590000000004</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.19027330000000001</v>
+      </c>
+      <c r="I15" s="30">
+        <v>1.742273E-8</v>
+      </c>
+      <c r="J15" s="12">
+        <v>2.4891650000000002E-4</v>
+      </c>
+      <c r="K15" s="20"/>
+      <c r="L15" s="21">
+        <v>0.90502150000000003</v>
+      </c>
+      <c r="M15" s="21">
+        <v>1</v>
+      </c>
+      <c r="N15" s="16">
+        <v>1.244583E-4</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0.99998856000000003</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0.99978460999999996</v>
+      </c>
+      <c r="T15" s="12">
+        <v>2.3693209999999999E-5</v>
+      </c>
+      <c r="U15" s="12">
+        <v>2.9589970000000001E-19</v>
+      </c>
+      <c r="V15" s="12">
+        <v>4.3579410000000002E-4</v>
+      </c>
+      <c r="W15" s="20"/>
+      <c r="X15" s="12">
+        <v>1.184661E-5</v>
+      </c>
+      <c r="Y15" s="12">
+        <v>1.4794979999999999E-19</v>
+      </c>
+      <c r="Z15" s="12">
+        <v>2.178971E-4</v>
+      </c>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="26">
+        <v>3.5848449999999997E-5</v>
+      </c>
+      <c r="AC15" s="23">
+        <v>3.5848449999999997E-5</v>
+      </c>
+      <c r="AD15" s="26">
+        <v>1.566708E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="27"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>